<commit_message>
update project plan and add category string to blog view
</commit_message>
<xml_diff>
--- a/Project Plan.xlsx
+++ b/Project Plan.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andypierce/Desktop/Development/PP4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A8F2950-1058-3346-92D4-9B57A9C27B93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A2DFB26-C4F5-5847-8711-36FB8DB80D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="50640" yWindow="-6440" windowWidth="48400" windowHeight="16940" xr2:uid="{872B3EE7-F43B-7649-AA18-AEB6D64C7670}"/>
+    <workbookView xWindow="44280" yWindow="-9120" windowWidth="48400" windowHeight="22720" activeTab="1" xr2:uid="{872B3EE7-F43B-7649-AA18-AEB6D64C7670}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="gant" sheetId="1" r:id="rId1"/>
+    <sheet name="user stories" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="82">
   <si>
     <t>User Stories</t>
   </si>
@@ -144,13 +145,301 @@
   </si>
   <si>
     <t>Refine comments and detail views</t>
+  </si>
+  <si>
+    <t>remove bookings that I cannot attend</t>
+  </si>
+  <si>
+    <t>Change bookings I have made</t>
+  </si>
+  <si>
+    <t>see what I have booked with the trainer</t>
+  </si>
+  <si>
+    <t>Review bookings I have made</t>
+  </si>
+  <si>
+    <t>check my details are correct</t>
+  </si>
+  <si>
+    <t>View my profile</t>
+  </si>
+  <si>
+    <t>Account Page</t>
+  </si>
+  <si>
+    <t>ask questions or ask for further information</t>
+  </si>
+  <si>
+    <t>Complete a contact form</t>
+  </si>
+  <si>
+    <t>arrange a session at a time that suits me</t>
+  </si>
+  <si>
+    <t>Book sessions</t>
+  </si>
+  <si>
+    <t>help me make a selection about what I want to book</t>
+  </si>
+  <si>
+    <t>See available sessions</t>
+  </si>
+  <si>
+    <t>show my appreciation for blog posts I like</t>
+  </si>
+  <si>
+    <t>Like a post</t>
+  </si>
+  <si>
+    <r>
+      <t>Approve comments: As a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF313131"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Site Admin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF313131"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> I can </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF313131"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>approve or disapprove comments</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF313131"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> so that </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF313131"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>I can filter out objectionable comments</t>
+    </r>
+  </si>
+  <si>
+    <t>ask questions, make comments or respond to other comments</t>
+  </si>
+  <si>
+    <t>Comment on a post</t>
+  </si>
+  <si>
+    <r>
+      <t>Create drafts: As a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF313131"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Site Admin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF313131"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> I can </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF313131"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>create draft posts</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF313131"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> so that </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF313131"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>I can finish writing the content later</t>
+    </r>
+  </si>
+  <si>
+    <t>find out about the subject of the blog</t>
+  </si>
+  <si>
+    <t>Access the detailed content of the blog</t>
+  </si>
+  <si>
+    <r>
+      <t>Manage posts: As a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF313131"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Site Admin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF313131"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> I can </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF313131"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>create, read, update and delete posts</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF313131"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> so that </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF313131"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>I can manage my blog content</t>
+    </r>
+  </si>
+  <si>
+    <t>select what I want to learn about</t>
+  </si>
+  <si>
+    <t>View a list of all blogs</t>
+  </si>
+  <si>
+    <t>book sessions</t>
+  </si>
+  <si>
+    <t>Create an account and sign in/out of the account</t>
+  </si>
+  <si>
+    <t>follow the site owner across avaialble platforms</t>
+  </si>
+  <si>
+    <t>Link to the users social media accounts</t>
+  </si>
+  <si>
+    <t>find out where sessions take place</t>
+  </si>
+  <si>
+    <t>View contact information and the location of services</t>
+  </si>
+  <si>
+    <t>ask questions or request further information</t>
+  </si>
+  <si>
+    <t>Conatct the site owner</t>
+  </si>
+  <si>
+    <t>arrange to train with the site owner</t>
+  </si>
+  <si>
+    <t>See available sessions and how to book them</t>
+  </si>
+  <si>
+    <t>see new blog posts that may interest me</t>
+  </si>
+  <si>
+    <t>View recently created content</t>
+  </si>
+  <si>
+    <t>select the page I need to interact with</t>
+  </si>
+  <si>
+    <t>Easily Navigate to the section I want</t>
+  </si>
+  <si>
+    <t>Welcome</t>
+  </si>
+  <si>
+    <t>Modules</t>
+  </si>
+  <si>
+    <t>so that I</t>
+  </si>
+  <si>
+    <t>I can</t>
+  </si>
+  <si>
+    <t>so that I can</t>
+  </si>
+  <si>
+    <t>ADMIN</t>
+  </si>
+  <si>
+    <t>As a</t>
+  </si>
+  <si>
+    <t>USER</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -175,8 +464,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF313131"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF313131"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -207,6 +524,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -220,7 +555,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -228,6 +563,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -544,8 +894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4103B497-E581-4047-BB96-77C66CC9C13A}">
   <dimension ref="A1:Y36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -716,7 +1066,7 @@
       <c r="B12" t="s">
         <v>7</v>
       </c>
-      <c r="H12" s="2"/>
+      <c r="H12" s="6"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -890,4 +1240,300 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{876B9BE3-52DE-684D-9F94-1E80DEA97083}">
+  <dimension ref="A1:G42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="4.1640625" style="9" customWidth="1"/>
+    <col min="3" max="4" width="70.5" style="8" customWidth="1"/>
+    <col min="5" max="5" width="5.33203125" customWidth="1"/>
+    <col min="6" max="7" width="70.5" style="7" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="12"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="12"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="9">
+        <v>1</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B6" s="9">
+        <v>2</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B8" s="9">
+        <v>3</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B10" s="9">
+        <v>4</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B12" s="9">
+        <v>5</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B14" s="9">
+        <v>6</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B16" s="9">
+        <v>7</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="20" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="9">
+        <v>8</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="20" x14ac:dyDescent="0.2">
+      <c r="B20" s="9">
+        <v>9</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="20" x14ac:dyDescent="0.2">
+      <c r="B22" s="9">
+        <v>10</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B24" s="9">
+        <v>11</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="9">
+        <v>12</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B28" s="9">
+        <v>13</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="9">
+        <v>14</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" s="9">
+        <v>15</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B34" s="9">
+        <v>16</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B36" s="9">
+        <v>17</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="C37" s="10"/>
+    </row>
+    <row r="38" spans="2:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="C38" s="10"/>
+    </row>
+    <row r="39" spans="2:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="C39" s="10"/>
+    </row>
+    <row r="40" spans="2:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="C40" s="10"/>
+    </row>
+    <row r="41" spans="2:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="C41" s="10"/>
+    </row>
+    <row r="42" spans="2:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="C42" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
center text and img in blog detail
</commit_message>
<xml_diff>
--- a/Project Plan.xlsx
+++ b/Project Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andypierce/Desktop/Development/PP4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A2DFB26-C4F5-5847-8711-36FB8DB80D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0648996D-0587-BC44-A807-05799C35FA7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44280" yWindow="-9120" windowWidth="48400" windowHeight="22720" activeTab="1" xr2:uid="{872B3EE7-F43B-7649-AA18-AEB6D64C7670}"/>
+    <workbookView xWindow="44280" yWindow="-9120" windowWidth="48400" windowHeight="22720" xr2:uid="{872B3EE7-F43B-7649-AA18-AEB6D64C7670}"/>
   </bookViews>
   <sheets>
     <sheet name="gant" sheetId="1" r:id="rId1"/>
@@ -894,8 +894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4103B497-E581-4047-BB96-77C66CC9C13A}">
   <dimension ref="A1:Y36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1075,7 +1075,7 @@
       <c r="B13" t="s">
         <v>8</v>
       </c>
-      <c r="I13" s="2"/>
+      <c r="I13" s="6"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -1084,7 +1084,7 @@
       <c r="B14" t="s">
         <v>9</v>
       </c>
-      <c r="I14" s="2"/>
+      <c r="I14" s="6"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -1246,7 +1246,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{876B9BE3-52DE-684D-9F94-1E80DEA97083}">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add map and contact info
</commit_message>
<xml_diff>
--- a/Project Plan.xlsx
+++ b/Project Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andypierce/Desktop/Development/PP4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0648996D-0587-BC44-A807-05799C35FA7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE8BF591-4BFE-C146-9E00-BE4CC0E6297C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="44280" yWindow="-9120" windowWidth="48400" windowHeight="22720" xr2:uid="{872B3EE7-F43B-7649-AA18-AEB6D64C7670}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="82">
   <si>
     <t>User Stories</t>
   </si>
@@ -126,19 +126,10 @@
     <t>Check project docs to confirm all areas are covered</t>
   </si>
   <si>
-    <t>Shop</t>
-  </si>
-  <si>
-    <t>if time allows</t>
-  </si>
-  <si>
     <t>PP4 Project plan</t>
   </si>
   <si>
     <t>Contact</t>
-  </si>
-  <si>
-    <t>Optional</t>
   </si>
   <si>
     <t>Sam to design Images</t>
@@ -434,12 +425,21 @@
   <si>
     <t>USER</t>
   </si>
+  <si>
+    <t>add contact me link to hompage</t>
+  </si>
+  <si>
+    <t>add info section to homepage</t>
+  </si>
+  <si>
+    <t>add social links to footer</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -450,15 +450,6 @@
     <font>
       <b/>
       <sz val="24"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -555,27 +546,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -895,7 +885,7 @@
   <dimension ref="A1:Y36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -913,7 +903,7 @@
   <sheetData>
     <row r="1" spans="1:25" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
@@ -994,7 +984,7 @@
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="6"/>
+      <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -1003,7 +993,7 @@
       <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="2"/>
+      <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -1012,16 +1002,16 @@
       <c r="B5" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="2"/>
+      <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -1030,7 +1020,7 @@
       <c r="B7" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="2"/>
+      <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -1039,7 +1029,7 @@
       <c r="B8" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="2"/>
+      <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -1048,16 +1038,16 @@
       <c r="B9" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="2"/>
+      <c r="I9" s="2"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
-      </c>
-      <c r="H11" s="2"/>
+        <v>32</v>
+      </c>
+      <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -1066,7 +1056,7 @@
       <c r="B12" t="s">
         <v>7</v>
       </c>
-      <c r="H12" s="6"/>
+      <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -1075,7 +1065,7 @@
       <c r="B13" t="s">
         <v>8</v>
       </c>
-      <c r="I13" s="6"/>
+      <c r="I13" s="5"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -1084,158 +1074,168 @@
       <c r="B14" t="s">
         <v>9</v>
       </c>
-      <c r="I14" s="6"/>
+      <c r="I14" s="5"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
-      </c>
-      <c r="J16" s="2"/>
+        <v>79</v>
+      </c>
+      <c r="I16" s="2"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
-      </c>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="3"/>
-      <c r="R17" s="3"/>
+        <v>80</v>
+      </c>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" t="s">
+        <v>81</v>
+      </c>
+      <c r="I18" s="2"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
-      </c>
-      <c r="K19" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="J19" s="2"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>12</v>
-      </c>
-      <c r="K20" s="2"/>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>10</v>
-      </c>
-      <c r="B21" t="s">
-        <v>13</v>
-      </c>
-      <c r="N21" s="2"/>
+        <v>31</v>
+      </c>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
-      </c>
-      <c r="N22" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="K22" s="2"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>10</v>
       </c>
       <c r="B23" t="s">
-        <v>15</v>
-      </c>
-      <c r="O23" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="K23" s="2"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" t="s">
+        <v>13</v>
+      </c>
+      <c r="N24" s="2"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B25" t="s">
-        <v>17</v>
-      </c>
-      <c r="P25" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="N25" s="2"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" t="s">
+        <v>15</v>
+      </c>
+      <c r="O26" s="2"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>16</v>
       </c>
-      <c r="B26" t="s">
-        <v>18</v>
-      </c>
-      <c r="P26" s="2"/>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>16</v>
-      </c>
-      <c r="B27" t="s">
-        <v>19</v>
-      </c>
-      <c r="P27" s="2"/>
+      <c r="B28" t="s">
+        <v>17</v>
+      </c>
+      <c r="P28" s="2"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B29" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q29" s="2"/>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>20</v>
-      </c>
-      <c r="B31" t="s">
-        <v>21</v>
-      </c>
-      <c r="R31" s="2"/>
+        <v>18</v>
+      </c>
+      <c r="P29" s="2"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" t="s">
+        <v>19</v>
+      </c>
+      <c r="P30" s="2"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q32" s="2"/>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>20</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B34" t="s">
+        <v>21</v>
+      </c>
+      <c r="R34" s="2"/>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35" t="s">
         <v>22</v>
       </c>
-      <c r="R32" s="2"/>
-    </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="R35" s="2"/>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>25</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B36" t="s">
         <v>26</v>
       </c>
-      <c r="U33" s="2"/>
-    </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A35" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>29</v>
-      </c>
-      <c r="B36" t="s">
-        <v>30</v>
-      </c>
-      <c r="V36" s="2"/>
-      <c r="W36" s="2"/>
-      <c r="X36" s="2"/>
-      <c r="Y36" s="2"/>
+      <c r="U36" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1253,285 +1253,285 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="4.1640625" style="9" customWidth="1"/>
-    <col min="3" max="4" width="70.5" style="8" customWidth="1"/>
+    <col min="2" max="2" width="4.1640625" style="8" customWidth="1"/>
+    <col min="3" max="4" width="70.5" style="7" customWidth="1"/>
     <col min="5" max="5" width="5.33203125" customWidth="1"/>
-    <col min="6" max="7" width="70.5" style="7" customWidth="1"/>
+    <col min="6" max="7" width="70.5" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="12"/>
-      <c r="B1" s="15"/>
-      <c r="C1" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>79</v>
+      <c r="A1" s="11"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="12"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>76</v>
+      <c r="A2" s="11"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
+      <c r="A3" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="12"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B4" s="9">
+        <v>71</v>
+      </c>
+      <c r="B4" s="8">
         <v>1</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>72</v>
+      <c r="C4" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B6" s="9">
+      <c r="B6" s="8">
         <v>2</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>70</v>
+      <c r="C6" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B8" s="9">
+      <c r="B8" s="8">
         <v>3</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>68</v>
+      <c r="C8" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B10" s="9">
+      <c r="B10" s="8">
         <v>4</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>66</v>
+      <c r="C10" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B12" s="9">
+      <c r="B12" s="8">
         <v>5</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>64</v>
+      <c r="C12" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B14" s="9">
+      <c r="B14" s="8">
         <v>6</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>62</v>
+      <c r="C14" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B16" s="9">
+      <c r="B16" s="8">
         <v>7</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>60</v>
+      <c r="C16" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>1</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18" s="8">
         <v>8</v>
       </c>
-      <c r="C18" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>57</v>
+      <c r="C18" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="20" x14ac:dyDescent="0.2">
-      <c r="B20" s="9">
+      <c r="B20" s="8">
         <v>9</v>
       </c>
-      <c r="C20" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>54</v>
+      <c r="C20" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="20" x14ac:dyDescent="0.2">
-      <c r="B22" s="9">
+      <c r="B22" s="8">
         <v>10</v>
       </c>
-      <c r="C22" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>51</v>
+      <c r="C22" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B24" s="9">
+      <c r="B24" s="8">
         <v>11</v>
       </c>
-      <c r="C24" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>49</v>
+      <c r="C24" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>2</v>
       </c>
-      <c r="B26" s="9">
+      <c r="B26" s="8">
         <v>12</v>
       </c>
-      <c r="C26" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>47</v>
+      <c r="C26" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B28" s="9">
+      <c r="B28" s="8">
         <v>13</v>
       </c>
-      <c r="C28" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>45</v>
+      <c r="C28" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>32</v>
-      </c>
-      <c r="B30" s="9">
+        <v>30</v>
+      </c>
+      <c r="B30" s="8">
         <v>14</v>
       </c>
-      <c r="C30" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>43</v>
+      <c r="C30" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>42</v>
-      </c>
-      <c r="B32" s="9">
+        <v>39</v>
+      </c>
+      <c r="B32" s="8">
         <v>15</v>
       </c>
-      <c r="C32" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>40</v>
+      <c r="C32" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B34" s="9">
+      <c r="B34" s="8">
         <v>16</v>
       </c>
-      <c r="C34" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>38</v>
+      <c r="C34" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B36" s="9">
+      <c r="B36" s="8">
         <v>17</v>
       </c>
-      <c r="C36" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>36</v>
+      <c r="C36" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="C37" s="10"/>
+      <c r="C37" s="9"/>
     </row>
     <row r="38" spans="2:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="C38" s="10"/>
+      <c r="C38" s="9"/>
     </row>
     <row r="39" spans="2:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="C39" s="10"/>
+      <c r="C39" s="9"/>
     </row>
     <row r="40" spans="2:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="C40" s="10"/>
+      <c r="C40" s="9"/>
     </row>
     <row r="41" spans="2:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="C41" s="10"/>
+      <c r="C41" s="9"/>
     </row>
     <row r="42" spans="2:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="C42" s="10"/>
+      <c r="C42" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add booking and session models and start welcome view
</commit_message>
<xml_diff>
--- a/Project Plan.xlsx
+++ b/Project Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andypierce/Desktop/Development/PP4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE8BF591-4BFE-C146-9E00-BE4CC0E6297C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE13DABB-3A0D-8C4C-97DB-C37C7B838DF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="44280" yWindow="-9120" windowWidth="48400" windowHeight="22720" xr2:uid="{872B3EE7-F43B-7649-AA18-AEB6D64C7670}"/>
   </bookViews>
@@ -93,9 +93,6 @@
     <t>Design simple contact form with map and details</t>
   </si>
   <si>
-    <t>Add Js verification</t>
-  </si>
-  <si>
     <t>email form and show confirmation message</t>
   </si>
   <si>
@@ -433,6 +430,9 @@
   </si>
   <si>
     <t>add social links to footer</t>
+  </si>
+  <si>
+    <t>Add verification</t>
   </si>
 </sst>
 </file>
@@ -882,10 +882,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4103B497-E581-4047-BB96-77C66CC9C13A}">
-  <dimension ref="A1:Y36"/>
+  <dimension ref="A1:Y30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -903,7 +903,7 @@
   <sheetData>
     <row r="1" spans="1:25" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
@@ -988,254 +988,256 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="I4" s="2"/>
+        <v>31</v>
+      </c>
+      <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="I5" s="2"/>
+        <v>7</v>
+      </c>
+      <c r="H5" s="5"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6" s="2"/>
+        <v>8</v>
+      </c>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="I7" s="2"/>
+        <v>9</v>
+      </c>
+      <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="I8" s="2"/>
+        <v>78</v>
+      </c>
+      <c r="I8" s="5"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
-      </c>
-      <c r="I9" s="2"/>
+        <v>79</v>
+      </c>
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>80</v>
+      </c>
+      <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
-      </c>
-      <c r="H11" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
-      </c>
-      <c r="H12" s="5"/>
+        <v>81</v>
+      </c>
+      <c r="I12" s="5"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="I13" s="5"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
-      </c>
-      <c r="I14" s="5"/>
+        <v>11</v>
+      </c>
+      <c r="J14" s="2"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>79</v>
-      </c>
-      <c r="I16" s="2"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>80</v>
-      </c>
-      <c r="I17" s="2"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>81</v>
-      </c>
-      <c r="I18" s="2"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="N18" s="2"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
-      </c>
-      <c r="J19" s="2"/>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" t="s">
+        <v>15</v>
+      </c>
+      <c r="O20" s="2"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
+      <c r="P21" s="2"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+      <c r="U24" s="2"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1</v>
+      </c>
+      <c r="U25" s="2"/>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>2</v>
+      </c>
+      <c r="U26" s="2"/>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" t="s">
+        <v>29</v>
+      </c>
+      <c r="U27" s="2"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" t="s">
         <v>3</v>
       </c>
-      <c r="B20" t="s">
-        <v>31</v>
-      </c>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="3"/>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>10</v>
-      </c>
-      <c r="B22" t="s">
-        <v>11</v>
-      </c>
-      <c r="K22" s="2"/>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" t="s">
-        <v>12</v>
-      </c>
-      <c r="K23" s="2"/>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>10</v>
-      </c>
-      <c r="B24" t="s">
-        <v>13</v>
-      </c>
-      <c r="N24" s="2"/>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>10</v>
-      </c>
-      <c r="B25" t="s">
-        <v>14</v>
-      </c>
-      <c r="N25" s="2"/>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>10</v>
-      </c>
-      <c r="B26" t="s">
-        <v>15</v>
-      </c>
-      <c r="O26" s="2"/>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>16</v>
-      </c>
-      <c r="B28" t="s">
-        <v>17</v>
-      </c>
-      <c r="P28" s="2"/>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="U28" s="2"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="B29" t="s">
-        <v>18</v>
-      </c>
-      <c r="P29" s="2"/>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="U29" s="2"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B30" t="s">
-        <v>19</v>
-      </c>
-      <c r="P30" s="2"/>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>23</v>
-      </c>
-      <c r="B32" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q32" s="2"/>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>20</v>
-      </c>
-      <c r="B34" t="s">
-        <v>21</v>
-      </c>
-      <c r="R34" s="2"/>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>20</v>
-      </c>
-      <c r="B35" t="s">
-        <v>22</v>
-      </c>
-      <c r="R35" s="2"/>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>25</v>
-      </c>
-      <c r="B36" t="s">
-        <v>26</v>
-      </c>
-      <c r="U36" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="U30" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1263,39 +1265,39 @@
       <c r="A1" s="11"/>
       <c r="B1" s="14"/>
       <c r="C1" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>77</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>78</v>
       </c>
       <c r="E1" s="13"/>
       <c r="F1" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="11"/>
       <c r="B2" s="14"/>
       <c r="C2" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>74</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>75</v>
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="11"/>
@@ -1306,16 +1308,16 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B4" s="8">
         <v>1</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -1323,10 +1325,10 @@
         <v>2</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -1334,10 +1336,10 @@
         <v>3</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -1345,10 +1347,10 @@
         <v>4</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -1356,10 +1358,10 @@
         <v>5</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -1367,10 +1369,10 @@
         <v>6</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -1378,10 +1380,10 @@
         <v>7</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="20" x14ac:dyDescent="0.2">
@@ -1392,13 +1394,13 @@
         <v>8</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="20" x14ac:dyDescent="0.2">
@@ -1406,13 +1408,13 @@
         <v>9</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="20" x14ac:dyDescent="0.2">
@@ -1420,13 +1422,13 @@
         <v>10</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1434,10 +1436,10 @@
         <v>11</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -1448,10 +1450,10 @@
         <v>12</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -1459,38 +1461,38 @@
         <v>13</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" s="8">
         <v>14</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B32" s="8">
         <v>15</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
@@ -1498,10 +1500,10 @@
         <v>16</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
@@ -1509,10 +1511,10 @@
         <v>17</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="20" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
adjust styling of various images
</commit_message>
<xml_diff>
--- a/Project Plan.xlsx
+++ b/Project Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andypierce/Desktop/Development/PP4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE13DABB-3A0D-8C4C-97DB-C37C7B838DF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662EA83A-4F21-E448-B1ED-47685D28C3A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44280" yWindow="-9120" windowWidth="48400" windowHeight="22720" xr2:uid="{872B3EE7-F43B-7649-AA18-AEB6D64C7670}"/>
+    <workbookView xWindow="30240" yWindow="-1460" windowWidth="38400" windowHeight="19520" xr2:uid="{872B3EE7-F43B-7649-AA18-AEB6D64C7670}"/>
   </bookViews>
   <sheets>
     <sheet name="gant" sheetId="1" r:id="rId1"/>
@@ -885,7 +885,7 @@
   <dimension ref="A1:Y30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1083,7 +1083,7 @@
       <c r="B14" t="s">
         <v>11</v>
       </c>
-      <c r="J14" s="2"/>
+      <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -1092,7 +1092,7 @@
       <c r="B15" t="s">
         <v>12</v>
       </c>
-      <c r="J15" s="2"/>
+      <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -1101,7 +1101,7 @@
       <c r="B16" t="s">
         <v>13</v>
       </c>
-      <c r="K16" s="2"/>
+      <c r="K16" s="5"/>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -1110,7 +1110,7 @@
       <c r="B17" t="s">
         <v>14</v>
       </c>
-      <c r="K17" s="2"/>
+      <c r="K17" s="5"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
@@ -1128,10 +1128,6 @@
       <c r="B19" t="s">
         <v>30</v>
       </c>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
       <c r="P19" s="3"/>

</xml_diff>

<commit_message>
fix bug on likes
</commit_message>
<xml_diff>
--- a/Project Plan.xlsx
+++ b/Project Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andypierce/Desktop/Development/PP4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662EA83A-4F21-E448-B1ED-47685D28C3A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3A39B91-3714-8248-BFBB-CF08D6EE0CFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30240" yWindow="-1460" windowWidth="38400" windowHeight="19520" xr2:uid="{872B3EE7-F43B-7649-AA18-AEB6D64C7670}"/>
   </bookViews>
@@ -885,7 +885,7 @@
   <dimension ref="A1:Y30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="U24" sqref="U24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1119,7 +1119,7 @@
       <c r="B18" t="s">
         <v>6</v>
       </c>
-      <c r="N18" s="2"/>
+      <c r="N18" s="5"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
@@ -1141,7 +1141,7 @@
       <c r="B20" t="s">
         <v>15</v>
       </c>
-      <c r="O20" s="2"/>
+      <c r="O20" s="5"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" t="s">

</xml_diff>

<commit_message>
add send email function on booking creation
</commit_message>
<xml_diff>
--- a/Project Plan.xlsx
+++ b/Project Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andypierce/Desktop/Development/PP4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3A39B91-3714-8248-BFBB-CF08D6EE0CFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C0641C-2516-5548-A1F6-46EAD6BC2C87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30240" yWindow="-1460" windowWidth="38400" windowHeight="19520" xr2:uid="{872B3EE7-F43B-7649-AA18-AEB6D64C7670}"/>
   </bookViews>
@@ -885,7 +885,7 @@
   <dimension ref="A1:Y30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U24" sqref="U24"/>
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1150,7 +1150,7 @@
       <c r="B21" t="s">
         <v>23</v>
       </c>
-      <c r="P21" s="2"/>
+      <c r="P21" s="5"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" t="s">

</xml_diff>